<commit_message>
A very minimal admin dashboard added
</commit_message>
<xml_diff>
--- a/EmployeeManagementSystemDemoData.xlsx
+++ b/EmployeeManagementSystemDemoData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\csharprepo\EmployeeManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDF63E0-7C8D-411A-A0D2-1E5032B5625B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73E1847-DF40-48F2-8A82-B2996305F9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="6" xr2:uid="{A2C0B584-E66D-4AF2-B748-8611E1416A2B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{A2C0B584-E66D-4AF2-B748-8611E1416A2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Departments" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Production</t>
   </si>
   <si>
-    <t>Marketting</t>
-  </si>
-  <si>
     <t>DesignationName</t>
   </si>
   <si>
@@ -156,10 +153,34 @@
     <t>ExpiryDate</t>
   </si>
   <si>
-    <t>RoleName</t>
-  </si>
-  <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Ashish</t>
+  </si>
+  <si>
+    <t>Sapkota</t>
+  </si>
+  <si>
+    <t>ashishspkt6566@gmail.com</t>
+  </si>
+  <si>
+    <t>JanashittalPath Tole, Bharatpur-10</t>
+  </si>
+  <si>
+    <t>Due to traffic jam in Chitwan National Park</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Nopassword</t>
+  </si>
+  <si>
+    <t>aacsspkt3@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -518,7 +539,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -577,7 +598,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D6"/>
+      <selection activeCell="C15" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,13 +614,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -607,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -621,7 +642,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -635,7 +656,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>4</v>
@@ -649,7 +670,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -663,7 +684,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -679,10 +700,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E695733-7A92-4AE8-B321-612EBFD98109}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,7 +716,7 @@
     <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -705,37 +726,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
         <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -743,28 +764,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
       </c>
       <c r="E2">
         <v>9824277417</v>
       </c>
       <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
       </c>
       <c r="J2" s="1">
         <v>44197</v>
@@ -774,6 +795,44 @@
       </c>
       <c r="L2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>19819276566</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="1">
+        <v>44371</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -783,19 +842,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C391B0A3-894C-453F-87C1-81291933DA5F}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -803,16 +862,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -826,10 +885,27 @@
         <v>44365</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44357</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -839,10 +915,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1385F0CA-17DD-4012-AE67-27F01C10C7BE}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,16 +935,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
         <v>36</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -886,6 +962,23 @@
       </c>
       <c r="E2">
         <v>12000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>8500</v>
       </c>
     </row>
   </sheetData>
@@ -897,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1D9915-F29F-418B-BBA0-FB11A4D2D223}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,16 +1008,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -951,26 +1044,31 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6EAB459-6BD1-4516-BBFD-E8AC130D26BA}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -978,13 +1076,27 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>